<commit_message>
Modification on controlling interface
</commit_message>
<xml_diff>
--- a/RoboRTS-Firmware-master/Parameters.xlsx
+++ b/RoboRTS-Firmware-master/Parameters.xlsx
@@ -3,13 +3,14 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D407B05-C9A1-4590-A304-BEDE770B2923}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{155432AC-8993-4476-9AA6-34DFFE9C190B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12440" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="sys_config.h" sheetId="1" r:id="rId1"/>
     <sheet name="Gimbal_PID" sheetId="2" r:id="rId2"/>
+    <sheet name="Chassis_Position" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -21,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="96">
   <si>
     <t>Parameter</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -309,6 +310,58 @@
   </si>
   <si>
     <t>speed_y_kd</t>
+  </si>
+  <si>
+    <t>pid_spd</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>pid_chassis_angle</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>kp</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ki</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>kd</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Date</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>maxout</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>intergral_limit</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>&gt;300 = 5000 rmp</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Note</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>These parameters are at the line 332, 336 in chassis_task.c</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2200.0f</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>3000.0f</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -368,7 +421,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -389,16 +442,54 @@
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="11">
+  <dxfs count="15">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -754,8 +845,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AJ13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L5" sqref="L5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -1203,33 +1294,143 @@
         <v>50</v>
       </c>
     </row>
+    <row r="5" spans="1:36" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="3">
+        <v>43549</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="D5" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="E5" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="F5" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="G5" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="H5" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="I5" s="7" t="s">
+        <v>95</v>
+      </c>
+      <c r="J5" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="K5" s="7" t="s">
+        <v>95</v>
+      </c>
+      <c r="L5" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="M5" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="N5" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="O5" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="P5" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q5" s="7">
+        <v>2500</v>
+      </c>
+      <c r="R5" s="7">
+        <v>2000</v>
+      </c>
+      <c r="S5" s="7">
+        <v>76</v>
+      </c>
+      <c r="T5" s="7">
+        <v>478</v>
+      </c>
+      <c r="U5" s="7">
+        <v>445</v>
+      </c>
+      <c r="V5" s="7">
+        <v>345</v>
+      </c>
+      <c r="W5" s="7">
+        <v>0</v>
+      </c>
+      <c r="X5" s="7">
+        <v>0</v>
+      </c>
+      <c r="Y5" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="Z5" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="AA5" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="AB5" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="AC5" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="AD5" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="AE5" s="7">
+        <v>20</v>
+      </c>
+      <c r="AF5" s="7">
+        <v>-20</v>
+      </c>
+      <c r="AG5" s="7">
+        <v>180</v>
+      </c>
+      <c r="AH5" s="7">
+        <v>-180</v>
+      </c>
+      <c r="AI5" s="7">
+        <v>300</v>
+      </c>
+      <c r="AJ5" s="7">
+        <v>50</v>
+      </c>
+    </row>
     <row r="9" spans="1:36" ht="14.15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="7" t="s">
+      <c r="A9" s="12" t="s">
         <v>67</v>
       </c>
-      <c r="B9" s="7"/>
-      <c r="C9" s="7"/>
+      <c r="B9" s="12"/>
+      <c r="C9" s="12"/>
     </row>
     <row r="10" spans="1:36" ht="14.15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="8" t="s">
+      <c r="A10" s="13" t="s">
         <v>68</v>
       </c>
-      <c r="B10" s="8"/>
-      <c r="C10" s="8"/>
+      <c r="B10" s="13"/>
+      <c r="C10" s="13"/>
     </row>
     <row r="11" spans="1:36" ht="14.15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="8" t="s">
+      <c r="A11" s="13" t="s">
         <v>69</v>
       </c>
-      <c r="B11" s="8"/>
-      <c r="C11" s="8"/>
+      <c r="B11" s="13"/>
+      <c r="C11" s="13"/>
     </row>
     <row r="12" spans="1:36" ht="14.15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="8" t="s">
+      <c r="A12" s="13" t="s">
         <v>70</v>
       </c>
-      <c r="B12" s="8"/>
-      <c r="C12" s="8"/>
+      <c r="B12" s="13"/>
+      <c r="C12" s="13"/>
     </row>
     <row r="13" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A13" s="1"/>
@@ -1245,28 +1446,53 @@
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="A4:XFD4">
-    <cfRule type="cellIs" dxfId="10" priority="5" operator="notEqual">
+    <cfRule type="cellIs" dxfId="14" priority="10" operator="notEqual">
       <formula>A3</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C4:F4">
-    <cfRule type="cellIs" dxfId="9" priority="4" operator="notEqual">
+    <cfRule type="cellIs" dxfId="13" priority="9" operator="notEqual">
       <formula>C3</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="U4">
-    <cfRule type="cellIs" dxfId="8" priority="3" operator="notEqual">
+    <cfRule type="cellIs" dxfId="12" priority="8" operator="notEqual">
       <formula>U3</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="V4">
-    <cfRule type="cellIs" dxfId="7" priority="2" operator="notEqual">
+    <cfRule type="cellIs" dxfId="11" priority="7" operator="notEqual">
       <formula>V3</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P4:T4">
-    <cfRule type="cellIs" dxfId="6" priority="1" operator="notEqual">
+    <cfRule type="cellIs" dxfId="10" priority="6" operator="notEqual">
       <formula>P3</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A5:XFD5">
+    <cfRule type="cellIs" dxfId="9" priority="5" operator="notEqual">
+      <formula>A4</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C5:F5">
+    <cfRule type="cellIs" dxfId="8" priority="4" operator="notEqual">
+      <formula>C4</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="U5">
+    <cfRule type="cellIs" dxfId="7" priority="3" operator="notEqual">
+      <formula>U4</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="V5">
+    <cfRule type="cellIs" dxfId="6" priority="2" operator="notEqual">
+      <formula>V4</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="P5:T5">
+    <cfRule type="cellIs" dxfId="5" priority="1" operator="notEqual">
+      <formula>P4</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1278,8 +1504,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:M5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -1465,26 +1691,210 @@
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="B4:XFD4">
-    <cfRule type="cellIs" dxfId="5" priority="5" operator="notEqual">
+    <cfRule type="cellIs" dxfId="4" priority="5" operator="notEqual">
       <formula>B3</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A4">
-    <cfRule type="cellIs" dxfId="4" priority="3" operator="notEqual">
+    <cfRule type="cellIs" dxfId="3" priority="3" operator="notEqual">
       <formula>A3</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B5:XFD5">
-    <cfRule type="cellIs" dxfId="1" priority="2" operator="notEqual">
+    <cfRule type="cellIs" dxfId="2" priority="2" operator="notEqual">
       <formula>B4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A5">
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="notEqual">
+    <cfRule type="cellIs" dxfId="1" priority="1" operator="notEqual">
       <formula>A4</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{44A0A821-D4A4-466C-BDEA-E447256B087A}">
+  <dimension ref="A1:O5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:M1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="9.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="2.08203125" customWidth="1"/>
+    <col min="13" max="13" width="15.83203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A1" s="14" t="s">
+        <v>93</v>
+      </c>
+      <c r="B1" s="14"/>
+      <c r="C1" s="14"/>
+      <c r="D1" s="14"/>
+      <c r="E1" s="14"/>
+      <c r="F1" s="14"/>
+      <c r="G1" s="14"/>
+      <c r="H1" s="14"/>
+      <c r="I1" s="14"/>
+      <c r="J1" s="14"/>
+      <c r="K1" s="14"/>
+      <c r="L1" s="14"/>
+      <c r="M1" s="14"/>
+      <c r="N1" s="10"/>
+      <c r="O1" s="10"/>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A2" s="14" t="s">
+        <v>88</v>
+      </c>
+      <c r="B2" s="14" t="s">
+        <v>83</v>
+      </c>
+      <c r="C2" s="14"/>
+      <c r="D2" s="14"/>
+      <c r="E2" s="14"/>
+      <c r="F2" s="14"/>
+      <c r="G2" s="14" t="s">
+        <v>84</v>
+      </c>
+      <c r="H2" s="14"/>
+      <c r="I2" s="14"/>
+      <c r="J2" s="14"/>
+      <c r="K2" s="14"/>
+      <c r="M2" s="14" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A3" s="14"/>
+      <c r="B3" t="s">
+        <v>89</v>
+      </c>
+      <c r="C3" t="s">
+        <v>90</v>
+      </c>
+      <c r="D3" t="s">
+        <v>85</v>
+      </c>
+      <c r="E3" t="s">
+        <v>86</v>
+      </c>
+      <c r="F3" t="s">
+        <v>87</v>
+      </c>
+      <c r="G3" t="s">
+        <v>89</v>
+      </c>
+      <c r="H3" t="s">
+        <v>90</v>
+      </c>
+      <c r="I3" t="s">
+        <v>85</v>
+      </c>
+      <c r="J3" t="s">
+        <v>86</v>
+      </c>
+      <c r="K3" t="s">
+        <v>87</v>
+      </c>
+      <c r="M3" s="14"/>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A4" s="8">
+        <v>43534</v>
+      </c>
+      <c r="B4">
+        <v>8000</v>
+      </c>
+      <c r="C4">
+        <v>500</v>
+      </c>
+      <c r="D4" s="11">
+        <v>4.5</v>
+      </c>
+      <c r="E4" s="11">
+        <v>0.05</v>
+      </c>
+      <c r="F4" s="11">
+        <v>0</v>
+      </c>
+      <c r="G4">
+        <v>300</v>
+      </c>
+      <c r="H4">
+        <v>50</v>
+      </c>
+      <c r="I4" s="11">
+        <v>14</v>
+      </c>
+      <c r="J4" s="11">
+        <v>0</v>
+      </c>
+      <c r="K4" s="11">
+        <v>50</v>
+      </c>
+      <c r="M4" s="9" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A5" s="8">
+        <v>43549</v>
+      </c>
+      <c r="B5">
+        <v>8000</v>
+      </c>
+      <c r="C5">
+        <v>500</v>
+      </c>
+      <c r="D5" s="11">
+        <v>4.5</v>
+      </c>
+      <c r="E5" s="11">
+        <v>0.05</v>
+      </c>
+      <c r="F5" s="11">
+        <v>0</v>
+      </c>
+      <c r="G5">
+        <v>300</v>
+      </c>
+      <c r="H5">
+        <v>50</v>
+      </c>
+      <c r="I5" s="11">
+        <v>10</v>
+      </c>
+      <c r="J5" s="11">
+        <v>0</v>
+      </c>
+      <c r="K5" s="11">
+        <v>50</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="5">
+    <mergeCell ref="B2:F2"/>
+    <mergeCell ref="G2:K2"/>
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="A1:M1"/>
+    <mergeCell ref="M2:M3"/>
+  </mergeCells>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <conditionalFormatting sqref="A5:K5">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="notEqual">
+      <formula>A4</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>